<commit_message>
feat: handle u shape graph
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -180,7 +180,7 @@
       <row>2</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -205,7 +205,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -230,7 +230,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -255,7 +255,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -280,7 +280,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -305,7 +305,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -330,7 +330,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -355,7 +355,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -380,7 +380,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="9" name="Image 9" descr="Picture"/>
@@ -405,7 +405,7 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="10" name="Image 10" descr="Picture"/>
@@ -430,7 +430,7 @@
       <row>12</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="11" name="Image 11" descr="Picture"/>
@@ -455,7 +455,7 @@
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="12" name="Image 12" descr="Picture"/>
@@ -480,7 +480,7 @@
       <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="13" name="Image 13" descr="Picture"/>
@@ -505,7 +505,7 @@
       <row>15</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="14" name="Image 14" descr="Picture"/>
@@ -530,7 +530,7 @@
       <row>16</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="15" name="Image 15" descr="Picture"/>
@@ -555,7 +555,7 @@
       <row>17</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="16" name="Image 16" descr="Picture"/>
@@ -580,7 +580,7 @@
       <row>18</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="17" name="Image 17" descr="Picture"/>
@@ -605,7 +605,7 @@
       <row>19</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="18" name="Image 18" descr="Picture"/>
@@ -630,7 +630,7 @@
       <row>20</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="19" name="Image 19" descr="Picture"/>
@@ -655,7 +655,7 @@
       <row>21</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="20" name="Image 20" descr="Picture"/>
@@ -680,7 +680,7 @@
       <row>22</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="21" name="Image 21" descr="Picture"/>
@@ -705,7 +705,7 @@
       <row>23</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="22" name="Image 22" descr="Picture"/>
@@ -730,7 +730,7 @@
       <row>24</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="23" name="Image 23" descr="Picture"/>
@@ -755,7 +755,7 @@
       <row>25</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="24" name="Image 24" descr="Picture"/>
@@ -780,7 +780,7 @@
       <row>26</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="25" name="Image 25" descr="Picture"/>
@@ -805,7 +805,7 @@
       <row>27</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="26" name="Image 26" descr="Picture"/>
@@ -830,7 +830,7 @@
       <row>28</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="27" name="Image 27" descr="Picture"/>
@@ -855,7 +855,7 @@
       <row>29</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="28" name="Image 28" descr="Picture"/>
@@ -880,7 +880,7 @@
       <row>30</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="29" name="Image 29" descr="Picture"/>
@@ -905,7 +905,7 @@
       <row>31</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="30" name="Image 30" descr="Picture"/>
@@ -930,7 +930,7 @@
       <row>32</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="31" name="Image 31" descr="Picture"/>
@@ -955,7 +955,7 @@
       <row>33</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="476250"/>
+    <ext cx="2286000" cy="762000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="32" name="Image 32" descr="Picture"/>
@@ -1332,7 +1332,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="120" customHeight="1">
+    <row r="3" ht="90" customHeight="1">
       <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
@@ -1341,11 +1341,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpkjot33x0.png</t>
-        </is>
-      </c>
+      <c r="C3" s="4" t="inlineStr"/>
       <c r="D3" s="3" t="n">
         <v>0</v>
       </c>
@@ -1362,7 +1358,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="120" customHeight="1">
+    <row r="4" ht="90" customHeight="1">
       <c r="A4" s="5" t="n">
         <v>2</v>
       </c>
@@ -1371,11 +1367,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpkzisgbdc.png</t>
-        </is>
-      </c>
+      <c r="C4" s="6" t="inlineStr"/>
       <c r="D4" s="5" t="n">
         <v>0</v>
       </c>
@@ -1392,7 +1384,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="120" customHeight="1">
+    <row r="5" ht="90" customHeight="1">
       <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
@@ -1401,11 +1393,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp4_0bkqio.png</t>
-        </is>
-      </c>
+      <c r="C5" s="4" t="inlineStr"/>
       <c r="D5" s="3" t="n">
         <v>0</v>
       </c>
@@ -1422,7 +1410,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="120" customHeight="1">
+    <row r="6" ht="90" customHeight="1">
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
@@ -1431,11 +1419,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpu8ni3_bi.png</t>
-        </is>
-      </c>
+      <c r="C6" s="6" t="inlineStr"/>
       <c r="D6" s="5" t="n">
         <v>0</v>
       </c>
@@ -1452,7 +1436,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="120" customHeight="1">
+    <row r="7" ht="90" customHeight="1">
       <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
@@ -1461,11 +1445,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpc1piukwg.png</t>
-        </is>
-      </c>
+      <c r="C7" s="4" t="inlineStr"/>
       <c r="D7" s="3" t="n">
         <v>0</v>
       </c>
@@ -1482,7 +1462,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="120" customHeight="1">
+    <row r="8" ht="90" customHeight="1">
       <c r="A8" s="5" t="n">
         <v>6</v>
       </c>
@@ -1491,11 +1471,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpjdk3ggpx.png</t>
-        </is>
-      </c>
+      <c r="C8" s="6" t="inlineStr"/>
       <c r="D8" s="5" t="n">
         <v>0</v>
       </c>
@@ -1512,7 +1488,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="120" customHeight="1">
+    <row r="9" ht="90" customHeight="1">
       <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
@@ -1521,11 +1497,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpdmw6soxh.png</t>
-        </is>
-      </c>
+      <c r="C9" s="4" t="inlineStr"/>
       <c r="D9" s="3" t="n">
         <v>0</v>
       </c>
@@ -1542,7 +1514,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="120" customHeight="1">
+    <row r="10" ht="90" customHeight="1">
       <c r="A10" s="5" t="n">
         <v>8</v>
       </c>
@@ -1551,11 +1523,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp7a2vu1f4.png</t>
-        </is>
-      </c>
+      <c r="C10" s="6" t="inlineStr"/>
       <c r="D10" s="5" t="n">
         <v>0</v>
       </c>
@@ -1572,7 +1540,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="120" customHeight="1">
+    <row r="11" ht="90" customHeight="1">
       <c r="A11" s="3" t="n">
         <v>9</v>
       </c>
@@ -1581,11 +1549,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpcpafjq26.png</t>
-        </is>
-      </c>
+      <c r="C11" s="4" t="inlineStr"/>
       <c r="D11" s="3" t="n">
         <v>0</v>
       </c>
@@ -1602,7 +1566,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="120" customHeight="1">
+    <row r="12" ht="90" customHeight="1">
       <c r="A12" s="5" t="n">
         <v>10</v>
       </c>
@@ -1611,11 +1575,7 @@
           <t>#9</t>
         </is>
       </c>
-      <c r="C12" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp12o5qzi0.png</t>
-        </is>
-      </c>
+      <c r="C12" s="6" t="inlineStr"/>
       <c r="D12" s="5" t="n">
         <v>0</v>
       </c>
@@ -1632,7 +1592,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="120" customHeight="1">
+    <row r="13" ht="90" customHeight="1">
       <c r="A13" s="3" t="n">
         <v>11</v>
       </c>
@@ -1641,11 +1601,7 @@
           <t>#8</t>
         </is>
       </c>
-      <c r="C13" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmptxku4o8a.png</t>
-        </is>
-      </c>
+      <c r="C13" s="4" t="inlineStr"/>
       <c r="D13" s="3" t="n">
         <v>0</v>
       </c>
@@ -1662,7 +1618,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="120" customHeight="1">
+    <row r="14" ht="90" customHeight="1">
       <c r="A14" s="5" t="n">
         <v>12</v>
       </c>
@@ -1671,11 +1627,7 @@
           <t>#7</t>
         </is>
       </c>
-      <c r="C14" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpbg3o3zl7.png</t>
-        </is>
-      </c>
+      <c r="C14" s="6" t="inlineStr"/>
       <c r="D14" s="5" t="n">
         <v>0</v>
       </c>
@@ -1692,7 +1644,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="120" customHeight="1">
+    <row r="15" ht="90" customHeight="1">
       <c r="A15" s="3" t="n">
         <v>13</v>
       </c>
@@ -1701,11 +1653,7 @@
           <t>#6</t>
         </is>
       </c>
-      <c r="C15" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpm4a9nheh.png</t>
-        </is>
-      </c>
+      <c r="C15" s="4" t="inlineStr"/>
       <c r="D15" s="3" t="n">
         <v>0</v>
       </c>
@@ -1722,7 +1670,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="120" customHeight="1">
+    <row r="16" ht="90" customHeight="1">
       <c r="A16" s="5" t="n">
         <v>14</v>
       </c>
@@ -1731,11 +1679,7 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C16" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp3e_rbkdf.png</t>
-        </is>
-      </c>
+      <c r="C16" s="6" t="inlineStr"/>
       <c r="D16" s="5" t="n">
         <v>0</v>
       </c>
@@ -1752,7 +1696,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="120" customHeight="1">
+    <row r="17" ht="90" customHeight="1">
       <c r="A17" s="3" t="n">
         <v>15</v>
       </c>
@@ -1761,11 +1705,7 @@
           <t>#4</t>
         </is>
       </c>
-      <c r="C17" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpn8fg6ut9.png</t>
-        </is>
-      </c>
+      <c r="C17" s="4" t="inlineStr"/>
       <c r="D17" s="3" t="n">
         <v>0</v>
       </c>
@@ -1782,7 +1722,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="120" customHeight="1">
+    <row r="18" ht="90" customHeight="1">
       <c r="A18" s="5" t="n">
         <v>16</v>
       </c>
@@ -1791,11 +1731,7 @@
           <t>#10</t>
         </is>
       </c>
-      <c r="C18" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp6g7199hz.png</t>
-        </is>
-      </c>
+      <c r="C18" s="6" t="inlineStr"/>
       <c r="D18" s="5" t="n">
         <v>0</v>
       </c>
@@ -1812,7 +1748,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="120" customHeight="1">
+    <row r="19" ht="90" customHeight="1">
       <c r="A19" s="3" t="n">
         <v>17</v>
       </c>
@@ -1821,11 +1757,7 @@
           <t>#3</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpf_897r10.png</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="inlineStr"/>
       <c r="D19" s="3" t="n">
         <v>0</v>
       </c>
@@ -1842,7 +1774,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="120" customHeight="1">
+    <row r="20" ht="90" customHeight="1">
       <c r="A20" s="5" t="n">
         <v>18</v>
       </c>
@@ -1851,11 +1783,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C20" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmplgeyonbu.png</t>
-        </is>
-      </c>
+      <c r="C20" s="6" t="inlineStr"/>
       <c r="D20" s="5" t="n">
         <v>0</v>
       </c>
@@ -1872,7 +1800,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="120" customHeight="1">
+    <row r="21" ht="90" customHeight="1">
       <c r="A21" s="3" t="n">
         <v>19</v>
       </c>
@@ -1881,11 +1809,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpkyq0z2gw.png</t>
-        </is>
-      </c>
+      <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" s="3" t="n">
         <v>0</v>
       </c>
@@ -1902,7 +1826,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="120" customHeight="1">
+    <row r="22" ht="90" customHeight="1">
       <c r="A22" s="5" t="n">
         <v>20</v>
       </c>
@@ -1911,11 +1835,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C22" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpkpruldth.png</t>
-        </is>
-      </c>
+      <c r="C22" s="6" t="inlineStr"/>
       <c r="D22" s="5" t="n">
         <v>0</v>
       </c>
@@ -1932,7 +1852,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="120" customHeight="1">
+    <row r="23" ht="90" customHeight="1">
       <c r="A23" s="3" t="n">
         <v>21</v>
       </c>
@@ -1941,11 +1861,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpsj_8y1f7.png</t>
-        </is>
-      </c>
+      <c r="C23" s="4" t="inlineStr"/>
       <c r="D23" s="3" t="n">
         <v>0</v>
       </c>
@@ -1962,7 +1878,7 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="120" customHeight="1">
+    <row r="24" ht="90" customHeight="1">
       <c r="A24" s="5" t="n">
         <v>22</v>
       </c>
@@ -1971,11 +1887,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C24" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpi3_xfytp.png</t>
-        </is>
-      </c>
+      <c r="C24" s="6" t="inlineStr"/>
       <c r="D24" s="5" t="n">
         <v>0</v>
       </c>
@@ -1992,7 +1904,7 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="120" customHeight="1">
+    <row r="25" ht="90" customHeight="1">
       <c r="A25" s="3" t="n">
         <v>23</v>
       </c>
@@ -2001,11 +1913,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C25" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp8g6s8y1c.png</t>
-        </is>
-      </c>
+      <c r="C25" s="4" t="inlineStr"/>
       <c r="D25" s="3" t="n">
         <v>0</v>
       </c>
@@ -2022,7 +1930,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="120" customHeight="1">
+    <row r="26" ht="90" customHeight="1">
       <c r="A26" s="5" t="n">
         <v>24</v>
       </c>
@@ -2031,11 +1939,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C26" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpurhf7by_.png</t>
-        </is>
-      </c>
+      <c r="C26" s="6" t="inlineStr"/>
       <c r="D26" s="5" t="n">
         <v>0</v>
       </c>
@@ -2052,7 +1956,7 @@
         </is>
       </c>
     </row>
-    <row r="27" ht="120" customHeight="1">
+    <row r="27" ht="90" customHeight="1">
       <c r="A27" s="3" t="n">
         <v>25</v>
       </c>
@@ -2061,11 +1965,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C27" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpfay604au.png</t>
-        </is>
-      </c>
+      <c r="C27" s="4" t="inlineStr"/>
       <c r="D27" s="3" t="n">
         <v>0</v>
       </c>
@@ -2082,7 +1982,7 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="120" customHeight="1">
+    <row r="28" ht="90" customHeight="1">
       <c r="A28" s="5" t="n">
         <v>26</v>
       </c>
@@ -2091,11 +1991,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C28" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpred9sr_0.png</t>
-        </is>
-      </c>
+      <c r="C28" s="6" t="inlineStr"/>
       <c r="D28" s="5" t="n">
         <v>0</v>
       </c>
@@ -2112,7 +2008,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="120" customHeight="1">
+    <row r="29" ht="90" customHeight="1">
       <c r="A29" s="3" t="n">
         <v>27</v>
       </c>
@@ -2121,11 +2017,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C29" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpod8p3we1.png</t>
-        </is>
-      </c>
+      <c r="C29" s="4" t="inlineStr"/>
       <c r="D29" s="3" t="n">
         <v>0</v>
       </c>
@@ -2142,7 +2034,7 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="120" customHeight="1">
+    <row r="30" ht="90" customHeight="1">
       <c r="A30" s="5" t="n">
         <v>28</v>
       </c>
@@ -2151,11 +2043,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C30" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp28uz_974.png</t>
-        </is>
-      </c>
+      <c r="C30" s="6" t="inlineStr"/>
       <c r="D30" s="5" t="n">
         <v>0</v>
       </c>
@@ -2172,7 +2060,7 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="120" customHeight="1">
+    <row r="31" ht="90" customHeight="1">
       <c r="A31" s="3" t="n">
         <v>29</v>
       </c>
@@ -2181,11 +2069,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C31" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpgyjjhkby.png</t>
-        </is>
-      </c>
+      <c r="C31" s="4" t="inlineStr"/>
       <c r="D31" s="3" t="n">
         <v>0</v>
       </c>
@@ -2202,7 +2086,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="120" customHeight="1">
+    <row r="32" ht="90" customHeight="1">
       <c r="A32" s="5" t="n">
         <v>30</v>
       </c>
@@ -2211,11 +2095,7 @@
           <t>#11</t>
         </is>
       </c>
-      <c r="C32" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpcr5s1aig.png</t>
-        </is>
-      </c>
+      <c r="C32" s="6" t="inlineStr"/>
       <c r="D32" s="5" t="n">
         <v>0</v>
       </c>
@@ -2232,7 +2112,7 @@
         </is>
       </c>
     </row>
-    <row r="33" ht="120" customHeight="1">
+    <row r="33" ht="90" customHeight="1">
       <c r="A33" s="3" t="n">
         <v>31</v>
       </c>
@@ -2241,11 +2121,7 @@
           <t>#9</t>
         </is>
       </c>
-      <c r="C33" s="4" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmpmqua_56h.png</t>
-        </is>
-      </c>
+      <c r="C33" s="4" t="inlineStr"/>
       <c r="D33" s="3" t="n">
         <v>0</v>
       </c>
@@ -2262,7 +2138,7 @@
         </is>
       </c>
     </row>
-    <row r="34" ht="120" customHeight="1">
+    <row r="34" ht="90" customHeight="1">
       <c r="A34" s="5" t="n">
         <v>32</v>
       </c>
@@ -2271,11 +2147,7 @@
           <t>#9</t>
         </is>
       </c>
-      <c r="C34" s="6" t="inlineStr">
-        <is>
-          <t>/var/folders/r8/420f3xv13xq21rkspncp85wr0000gn/T/tmp5cxp24ad.png</t>
-        </is>
-      </c>
+      <c r="C34" s="6" t="inlineStr"/>
       <c r="D34" s="5" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
feat: handle U and N shape
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -938,31 +938,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId31"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>2</col>
-      <colOff>0</colOff>
-      <row>33</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2286000" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="32" name="Image 32" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1265,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1338,7 +1313,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>#10</t>
+          <t>N#10</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr"/>
@@ -1450,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
@@ -1458,7 +1433,7 @@
       <c r="G7" s="3" t="inlineStr"/>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>折140#10-1000+1200x20</t>
+          <t>#10-510.5x11</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F8" s="5" t="n">
         <v>0</v>
@@ -1484,7 +1459,7 @@
       <c r="G8" s="5" t="inlineStr"/>
       <c r="H8" s="5" t="inlineStr">
         <is>
-          <t>#10-510.5x11</t>
+          <t>#10-550+21x5</t>
         </is>
       </c>
     </row>
@@ -1502,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
@@ -1510,7 +1485,7 @@
       <c r="G9" s="3" t="inlineStr"/>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>#10-550+21x5</t>
+          <t>#10-1000+1000x7</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1495,7 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>#10</t>
+          <t>#11</t>
         </is>
       </c>
       <c r="C10" s="6" t="inlineStr"/>
@@ -1528,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>0</v>
@@ -1536,7 +1511,7 @@
       <c r="G10" s="5" t="inlineStr"/>
       <c r="H10" s="5" t="inlineStr">
         <is>
-          <t>#10-1000+1000x7</t>
+          <t>#11-300x1</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1521,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>#11</t>
+          <t>#9</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr"/>
@@ -1562,7 +1537,7 @@
       <c r="G11" s="3" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>#11-300x1</t>
+          <t>#9-300x1</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1547,7 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>#9</t>
+          <t>#8</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr"/>
@@ -1588,7 +1563,7 @@
       <c r="G12" s="5" t="inlineStr"/>
       <c r="H12" s="5" t="inlineStr">
         <is>
-          <t>#9-300x1</t>
+          <t>#8-300x1</t>
         </is>
       </c>
     </row>
@@ -1598,7 +1573,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>#8</t>
+          <t>#7</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr"/>
@@ -1614,7 +1589,7 @@
       <c r="G13" s="3" t="inlineStr"/>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>#8-300x1</t>
+          <t>#7-300x1</t>
         </is>
       </c>
     </row>
@@ -1624,7 +1599,7 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>#7</t>
+          <t>#6</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr"/>
@@ -1640,7 +1615,7 @@
       <c r="G14" s="5" t="inlineStr"/>
       <c r="H14" s="5" t="inlineStr">
         <is>
-          <t>#7-300x1</t>
+          <t>#6-300x1</t>
         </is>
       </c>
     </row>
@@ -1650,7 +1625,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>#6</t>
+          <t>#5</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr"/>
@@ -1666,7 +1641,7 @@
       <c r="G15" s="3" t="inlineStr"/>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>#6-300x1</t>
+          <t>#5-300x1</t>
         </is>
       </c>
     </row>
@@ -1676,7 +1651,7 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>#5</t>
+          <t>#4</t>
         </is>
       </c>
       <c r="C16" s="6" t="inlineStr"/>
@@ -1692,7 +1667,7 @@
       <c r="G16" s="5" t="inlineStr"/>
       <c r="H16" s="5" t="inlineStr">
         <is>
-          <t>#5-300x1</t>
+          <t>#4-300x1</t>
         </is>
       </c>
     </row>
@@ -1702,7 +1677,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>#4</t>
+          <t>#10</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr"/>
@@ -1718,7 +1693,7 @@
       <c r="G17" s="3" t="inlineStr"/>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>#4-300x1</t>
+          <t>#10-300x1</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1703,7 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>#10</t>
+          <t>#3</t>
         </is>
       </c>
       <c r="C18" s="6" t="inlineStr"/>
@@ -1744,7 +1719,7 @@
       <c r="G18" s="5" t="inlineStr"/>
       <c r="H18" s="5" t="inlineStr">
         <is>
-          <t>#10-300x1</t>
+          <t>#3-300x1</t>
         </is>
       </c>
     </row>
@@ -1754,7 +1729,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>#3</t>
+          <t>#11</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr"/>
@@ -1770,7 +1745,7 @@
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>#3-300x1</t>
+          <t>#11-700x1</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1771,7 @@
       <c r="G20" s="5" t="inlineStr"/>
       <c r="H20" s="5" t="inlineStr">
         <is>
-          <t>#11-700x1</t>
+          <t>#11-500x1</t>
         </is>
       </c>
     </row>
@@ -1822,7 +1797,7 @@
       <c r="G21" s="3" t="inlineStr"/>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>#11-500x1</t>
+          <t>#11-60+1000x1</t>
         </is>
       </c>
     </row>
@@ -1848,7 +1823,7 @@
       <c r="G22" s="5" t="inlineStr"/>
       <c r="H22" s="5" t="inlineStr">
         <is>
-          <t>#11-60+1000x1</t>
+          <t>#11-60+500x1</t>
         </is>
       </c>
     </row>
@@ -1874,7 +1849,7 @@
       <c r="G23" s="3" t="inlineStr"/>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>#11-60+500x1</t>
+          <t>#11-600x1</t>
         </is>
       </c>
     </row>
@@ -1900,7 +1875,7 @@
       <c r="G24" s="5" t="inlineStr"/>
       <c r="H24" s="5" t="inlineStr">
         <is>
-          <t>#11-600x1</t>
+          <t>#11-60+1000+60x1</t>
         </is>
       </c>
     </row>
@@ -1926,7 +1901,7 @@
       <c r="G25" s="3" t="inlineStr"/>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>#11-60+1000+60x1</t>
+          <t>#11-60+500+60x1</t>
         </is>
       </c>
     </row>
@@ -1952,7 +1927,7 @@
       <c r="G26" s="5" t="inlineStr"/>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>#11-60+500+60x1</t>
+          <t>#11-700x1</t>
         </is>
       </c>
     </row>
@@ -2022,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>0</v>
@@ -2030,7 +2005,7 @@
       <c r="G29" s="3" t="inlineStr"/>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>#11-700x1</t>
+          <t>#11-60+700x6</t>
         </is>
       </c>
     </row>
@@ -2048,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F30" s="5" t="n">
         <v>0</v>
@@ -2056,7 +2031,7 @@
       <c r="G30" s="5" t="inlineStr"/>
       <c r="H30" s="5" t="inlineStr">
         <is>
-          <t>#11-60+700x6</t>
+          <t>#11-60+600x10</t>
         </is>
       </c>
     </row>
@@ -2074,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>0</v>
@@ -2082,7 +2057,7 @@
       <c r="G31" s="3" t="inlineStr"/>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>#11-60+600x10</t>
+          <t>#11-60+500x9</t>
         </is>
       </c>
     </row>
@@ -2092,7 +2067,7 @@
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>#11</t>
+          <t>#9</t>
         </is>
       </c>
       <c r="C32" s="6" t="inlineStr"/>
@@ -2100,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="F32" s="5" t="n">
         <v>0</v>
@@ -2108,7 +2083,7 @@
       <c r="G32" s="5" t="inlineStr"/>
       <c r="H32" s="5" t="inlineStr">
         <is>
-          <t>#11-60+500x9</t>
+          <t>#9-45+700x50</t>
         </is>
       </c>
     </row>
@@ -2133,32 +2108,6 @@
       </c>
       <c r="G33" s="3" t="inlineStr"/>
       <c r="H33" s="3" t="inlineStr">
-        <is>
-          <t>#9-45+700x50</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="90" customHeight="1">
-      <c r="A34" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" s="5" t="inlineStr">
-        <is>
-          <t>#9</t>
-        </is>
-      </c>
-      <c r="C34" s="6" t="inlineStr"/>
-      <c r="D34" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="5" t="inlineStr"/>
-      <c r="H34" s="5" t="inlineStr">
         <is>
           <t>#9-45+700x50</t>
         </is>

</xml_diff>

<commit_message>
feat: handle bent line
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -938,6 +938,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>33</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2286000" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="32" name="Image 32" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1240,7 +1265,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1425,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
@@ -1433,7 +1458,7 @@
       <c r="G7" s="3" t="inlineStr"/>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>#10-510.5x11</t>
+          <t>折140#10-1000+1200x20</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F8" s="5" t="n">
         <v>0</v>
@@ -1459,7 +1484,7 @@
       <c r="G8" s="5" t="inlineStr"/>
       <c r="H8" s="5" t="inlineStr">
         <is>
-          <t>#10-550+21x5</t>
+          <t>#10-510.5x11</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
@@ -1485,7 +1510,7 @@
       <c r="G9" s="3" t="inlineStr"/>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>#10-1000+1000x7</t>
+          <t>#10-550+21x5</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1520,7 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>#11</t>
+          <t>#10</t>
         </is>
       </c>
       <c r="C10" s="6" t="inlineStr"/>
@@ -1503,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>0</v>
@@ -1511,7 +1536,7 @@
       <c r="G10" s="5" t="inlineStr"/>
       <c r="H10" s="5" t="inlineStr">
         <is>
-          <t>#11-300x1</t>
+          <t>#10-1000+1000x7</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1546,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>#9</t>
+          <t>#11</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr"/>
@@ -1537,7 +1562,7 @@
       <c r="G11" s="3" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>#9-300x1</t>
+          <t>#11-300x1</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1572,7 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>#8</t>
+          <t>#9</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr"/>
@@ -1563,7 +1588,7 @@
       <c r="G12" s="5" t="inlineStr"/>
       <c r="H12" s="5" t="inlineStr">
         <is>
-          <t>#8-300x1</t>
+          <t>#9-300x1</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1598,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>#7</t>
+          <t>#8</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr"/>
@@ -1589,7 +1614,7 @@
       <c r="G13" s="3" t="inlineStr"/>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>#7-300x1</t>
+          <t>#8-300x1</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1624,7 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>#6</t>
+          <t>#7</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr"/>
@@ -1615,7 +1640,7 @@
       <c r="G14" s="5" t="inlineStr"/>
       <c r="H14" s="5" t="inlineStr">
         <is>
-          <t>#6-300x1</t>
+          <t>#7-300x1</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1650,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>#5</t>
+          <t>#6</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr"/>
@@ -1641,7 +1666,7 @@
       <c r="G15" s="3" t="inlineStr"/>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>#5-300x1</t>
+          <t>#6-300x1</t>
         </is>
       </c>
     </row>
@@ -1651,7 +1676,7 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>#4</t>
+          <t>#5</t>
         </is>
       </c>
       <c r="C16" s="6" t="inlineStr"/>
@@ -1667,7 +1692,7 @@
       <c r="G16" s="5" t="inlineStr"/>
       <c r="H16" s="5" t="inlineStr">
         <is>
-          <t>#4-300x1</t>
+          <t>#5-300x1</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1702,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>#10</t>
+          <t>#4</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr"/>
@@ -1693,7 +1718,7 @@
       <c r="G17" s="3" t="inlineStr"/>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>#10-300x1</t>
+          <t>#4-300x1</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1728,7 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>#3</t>
+          <t>#10</t>
         </is>
       </c>
       <c r="C18" s="6" t="inlineStr"/>
@@ -1719,7 +1744,7 @@
       <c r="G18" s="5" t="inlineStr"/>
       <c r="H18" s="5" t="inlineStr">
         <is>
-          <t>#3-300x1</t>
+          <t>#10-300x1</t>
         </is>
       </c>
     </row>
@@ -1729,7 +1754,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>#11</t>
+          <t>#3</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr"/>
@@ -1745,7 +1770,7 @@
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>#11-700x1</t>
+          <t>#3-300x1</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1796,7 @@
       <c r="G20" s="5" t="inlineStr"/>
       <c r="H20" s="5" t="inlineStr">
         <is>
-          <t>#11-500x1</t>
+          <t>#11-700x1</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1822,7 @@
       <c r="G21" s="3" t="inlineStr"/>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>#11-60+1000x1</t>
+          <t>#11-500x1</t>
         </is>
       </c>
     </row>
@@ -1823,7 +1848,7 @@
       <c r="G22" s="5" t="inlineStr"/>
       <c r="H22" s="5" t="inlineStr">
         <is>
-          <t>#11-60+500x1</t>
+          <t>#11-60+1000x1</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1874,7 @@
       <c r="G23" s="3" t="inlineStr"/>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>#11-600x1</t>
+          <t>#11-60+500x1</t>
         </is>
       </c>
     </row>
@@ -1875,7 +1900,7 @@
       <c r="G24" s="5" t="inlineStr"/>
       <c r="H24" s="5" t="inlineStr">
         <is>
-          <t>#11-60+1000+60x1</t>
+          <t>#11-600x1</t>
         </is>
       </c>
     </row>
@@ -1901,7 +1926,7 @@
       <c r="G25" s="3" t="inlineStr"/>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>#11-60+500+60x1</t>
+          <t>#11-60+1000+60x1</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1952,7 @@
       <c r="G26" s="5" t="inlineStr"/>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>#11-700x1</t>
+          <t>#11-60+500+60x1</t>
         </is>
       </c>
     </row>
@@ -1997,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F29" s="3" t="n">
         <v>0</v>
@@ -2005,7 +2030,7 @@
       <c r="G29" s="3" t="inlineStr"/>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>#11-60+700x6</t>
+          <t>#11-700x1</t>
         </is>
       </c>
     </row>
@@ -2023,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F30" s="5" t="n">
         <v>0</v>
@@ -2031,7 +2056,7 @@
       <c r="G30" s="5" t="inlineStr"/>
       <c r="H30" s="5" t="inlineStr">
         <is>
-          <t>#11-60+600x10</t>
+          <t>#11-60+700x6</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>0</v>
@@ -2057,7 +2082,7 @@
       <c r="G31" s="3" t="inlineStr"/>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>#11-60+500x9</t>
+          <t>#11-60+600x10</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2092,7 @@
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>#9</t>
+          <t>#11</t>
         </is>
       </c>
       <c r="C32" s="6" t="inlineStr"/>
@@ -2075,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="F32" s="5" t="n">
         <v>0</v>
@@ -2083,7 +2108,7 @@
       <c r="G32" s="5" t="inlineStr"/>
       <c r="H32" s="5" t="inlineStr">
         <is>
-          <t>#9-45+700x50</t>
+          <t>#11-60+500x9</t>
         </is>
       </c>
     </row>
@@ -2108,6 +2133,32 @@
       </c>
       <c r="G33" s="3" t="inlineStr"/>
       <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>#9-45+700x50</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="90" customHeight="1">
+      <c r="A34" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5" t="inlineStr">
+        <is>
+          <t>#9</t>
+        </is>
+      </c>
+      <c r="C34" s="6" t="inlineStr"/>
+      <c r="D34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F34" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5" t="inlineStr"/>
+      <c r="H34" s="5" t="inlineStr">
         <is>
           <t>#9-45+700x50</t>
         </is>

</xml_diff>

<commit_message>
fix: missing length and weight
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -1343,7 +1343,7 @@
       </c>
       <c r="C3" s="4" t="inlineStr"/>
       <c r="D3" s="3" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>31</v>
@@ -1369,13 +1369,13 @@
       </c>
       <c r="C4" s="6" t="inlineStr"/>
       <c r="D4" s="5" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0</v>
+        <v>19212</v>
       </c>
       <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
@@ -1395,13 +1395,13 @@
       </c>
       <c r="C5" s="4" t="inlineStr"/>
       <c r="D5" s="3" t="n">
-        <v>0</v>
+        <v>571</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>0</v>
+        <v>3657</v>
       </c>
       <c r="G5" s="3" t="inlineStr"/>
       <c r="H5" s="3" t="inlineStr">
@@ -1421,13 +1421,13 @@
       </c>
       <c r="C6" s="6" t="inlineStr"/>
       <c r="D6" s="5" t="n">
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>0</v>
+        <v>8966</v>
       </c>
       <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
@@ -1447,13 +1447,13 @@
       </c>
       <c r="C7" s="4" t="inlineStr"/>
       <c r="D7" s="3" t="n">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>14089</v>
       </c>
       <c r="G7" s="3" t="inlineStr"/>
       <c r="H7" s="3" t="inlineStr">
@@ -1473,13 +1473,13 @@
       </c>
       <c r="C8" s="6" t="inlineStr"/>
       <c r="D8" s="5" t="n">
-        <v>0</v>
+        <v>510</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>11</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0</v>
+        <v>3269</v>
       </c>
       <c r="G8" s="5" t="inlineStr"/>
       <c r="H8" s="5" t="inlineStr">
@@ -1499,13 +1499,13 @@
       </c>
       <c r="C9" s="4" t="inlineStr"/>
       <c r="D9" s="3" t="n">
-        <v>0</v>
+        <v>571</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>5</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>0</v>
+        <v>3657</v>
       </c>
       <c r="G9" s="3" t="inlineStr"/>
       <c r="H9" s="3" t="inlineStr">
@@ -1525,13 +1525,13 @@
       </c>
       <c r="C10" s="6" t="inlineStr"/>
       <c r="D10" s="5" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>7</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0</v>
+        <v>12808</v>
       </c>
       <c r="G10" s="5" t="inlineStr"/>
       <c r="H10" s="5" t="inlineStr">
@@ -1551,13 +1551,13 @@
       </c>
       <c r="C11" s="4" t="inlineStr"/>
       <c r="D11" s="3" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0</v>
+        <v>2372</v>
       </c>
       <c r="G11" s="3" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr">
@@ -1577,13 +1577,13 @@
       </c>
       <c r="C12" s="6" t="inlineStr"/>
       <c r="D12" s="5" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>0</v>
+        <v>1508</v>
       </c>
       <c r="G12" s="5" t="inlineStr"/>
       <c r="H12" s="5" t="inlineStr">
@@ -1603,13 +1603,13 @@
       </c>
       <c r="C13" s="4" t="inlineStr"/>
       <c r="D13" s="3" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>0</v>
+        <v>1192</v>
       </c>
       <c r="G13" s="3" t="inlineStr"/>
       <c r="H13" s="3" t="inlineStr">
@@ -1629,13 +1629,13 @@
       </c>
       <c r="C14" s="6" t="inlineStr"/>
       <c r="D14" s="5" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0</v>
+        <v>913</v>
       </c>
       <c r="G14" s="5" t="inlineStr"/>
       <c r="H14" s="5" t="inlineStr">
@@ -1655,13 +1655,13 @@
       </c>
       <c r="C15" s="4" t="inlineStr"/>
       <c r="D15" s="3" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>670</v>
       </c>
       <c r="G15" s="3" t="inlineStr"/>
       <c r="H15" s="3" t="inlineStr">
@@ -1681,13 +1681,13 @@
       </c>
       <c r="C16" s="6" t="inlineStr"/>
       <c r="D16" s="5" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>0</v>
+        <v>466</v>
       </c>
       <c r="G16" s="5" t="inlineStr"/>
       <c r="H16" s="5" t="inlineStr">
@@ -1707,13 +1707,13 @@
       </c>
       <c r="C17" s="4" t="inlineStr"/>
       <c r="D17" s="3" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E17" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>299</v>
       </c>
       <c r="G17" s="3" t="inlineStr"/>
       <c r="H17" s="3" t="inlineStr">
@@ -1733,13 +1733,13 @@
       </c>
       <c r="C18" s="6" t="inlineStr"/>
       <c r="D18" s="5" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0</v>
+        <v>1921</v>
       </c>
       <c r="G18" s="5" t="inlineStr"/>
       <c r="H18" s="5" t="inlineStr">
@@ -1759,13 +1759,13 @@
       </c>
       <c r="C19" s="4" t="inlineStr"/>
       <c r="D19" s="3" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="G19" s="3" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr">
@@ -1785,13 +1785,13 @@
       </c>
       <c r="C20" s="6" t="inlineStr"/>
       <c r="D20" s="5" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>0</v>
+        <v>5534</v>
       </c>
       <c r="G20" s="5" t="inlineStr"/>
       <c r="H20" s="5" t="inlineStr">
@@ -1811,13 +1811,13 @@
       </c>
       <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" s="3" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>0</v>
+        <v>3953</v>
       </c>
       <c r="G21" s="3" t="inlineStr"/>
       <c r="H21" s="3" t="inlineStr">
@@ -1837,13 +1837,13 @@
       </c>
       <c r="C22" s="6" t="inlineStr"/>
       <c r="D22" s="5" t="n">
-        <v>0</v>
+        <v>1060</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>0</v>
+        <v>8380</v>
       </c>
       <c r="G22" s="5" t="inlineStr"/>
       <c r="H22" s="5" t="inlineStr">
@@ -1863,13 +1863,13 @@
       </c>
       <c r="C23" s="4" t="inlineStr"/>
       <c r="D23" s="3" t="n">
-        <v>0</v>
+        <v>560</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>0</v>
+        <v>4427</v>
       </c>
       <c r="G23" s="3" t="inlineStr"/>
       <c r="H23" s="3" t="inlineStr">
@@ -1889,13 +1889,13 @@
       </c>
       <c r="C24" s="6" t="inlineStr"/>
       <c r="D24" s="5" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>0</v>
+        <v>4744</v>
       </c>
       <c r="G24" s="5" t="inlineStr"/>
       <c r="H24" s="5" t="inlineStr">
@@ -1915,13 +1915,13 @@
       </c>
       <c r="C25" s="4" t="inlineStr"/>
       <c r="D25" s="3" t="n">
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="n">
-        <v>0</v>
+        <v>8855</v>
       </c>
       <c r="G25" s="3" t="inlineStr"/>
       <c r="H25" s="3" t="inlineStr">
@@ -1941,13 +1941,13 @@
       </c>
       <c r="C26" s="6" t="inlineStr"/>
       <c r="D26" s="5" t="n">
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>0</v>
+        <v>4902</v>
       </c>
       <c r="G26" s="5" t="inlineStr"/>
       <c r="H26" s="5" t="inlineStr">
@@ -1967,13 +1967,13 @@
       </c>
       <c r="C27" s="4" t="inlineStr"/>
       <c r="D27" s="3" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F27" s="3" t="n">
-        <v>0</v>
+        <v>5534</v>
       </c>
       <c r="G27" s="3" t="inlineStr"/>
       <c r="H27" s="3" t="inlineStr">
@@ -1993,13 +1993,13 @@
       </c>
       <c r="C28" s="6" t="inlineStr"/>
       <c r="D28" s="5" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>0</v>
+        <v>5534</v>
       </c>
       <c r="G28" s="5" t="inlineStr"/>
       <c r="H28" s="5" t="inlineStr">
@@ -2019,13 +2019,13 @@
       </c>
       <c r="C29" s="4" t="inlineStr"/>
       <c r="D29" s="3" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="n">
-        <v>0</v>
+        <v>5534</v>
       </c>
       <c r="G29" s="3" t="inlineStr"/>
       <c r="H29" s="3" t="inlineStr">
@@ -2045,13 +2045,13 @@
       </c>
       <c r="C30" s="6" t="inlineStr"/>
       <c r="D30" s="5" t="n">
-        <v>0</v>
+        <v>760</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>6</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>0</v>
+        <v>6009</v>
       </c>
       <c r="G30" s="5" t="inlineStr"/>
       <c r="H30" s="5" t="inlineStr">
@@ -2071,13 +2071,13 @@
       </c>
       <c r="C31" s="4" t="inlineStr"/>
       <c r="D31" s="3" t="n">
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>10</v>
       </c>
       <c r="F31" s="3" t="n">
-        <v>0</v>
+        <v>5218</v>
       </c>
       <c r="G31" s="3" t="inlineStr"/>
       <c r="H31" s="3" t="inlineStr">
@@ -2097,13 +2097,13 @@
       </c>
       <c r="C32" s="6" t="inlineStr"/>
       <c r="D32" s="5" t="n">
-        <v>0</v>
+        <v>560</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>9</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>0</v>
+        <v>4427</v>
       </c>
       <c r="G32" s="5" t="inlineStr"/>
       <c r="H32" s="5" t="inlineStr">
@@ -2123,13 +2123,13 @@
       </c>
       <c r="C33" s="4" t="inlineStr"/>
       <c r="D33" s="3" t="n">
-        <v>0</v>
+        <v>745</v>
       </c>
       <c r="E33" s="3" t="n">
         <v>50</v>
       </c>
       <c r="F33" s="3" t="n">
-        <v>0</v>
+        <v>3744</v>
       </c>
       <c r="G33" s="3" t="inlineStr"/>
       <c r="H33" s="3" t="inlineStr">
@@ -2149,13 +2149,13 @@
       </c>
       <c r="C34" s="6" t="inlineStr"/>
       <c r="D34" s="5" t="n">
-        <v>0</v>
+        <v>745</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>50</v>
       </c>
       <c r="F34" s="5" t="n">
-        <v>0</v>
+        <v>3744</v>
       </c>
       <c r="G34" s="5" t="inlineStr"/>
       <c r="H34" s="5" t="inlineStr">

</xml_diff>

<commit_message>
chore: modify bent graphic ui
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -1680,7 +1680,7 @@
     <row r="16">
       <c r="A16" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 10:35:40 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 11:03:18 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
     <row r="17">
       <c r="A17" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 10:35:40 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 11:03:18 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2414,7 +2414,7 @@
     <row r="15">
       <c r="A15" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 10:35:41 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 11:03:19 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2703,7 +2703,7 @@
     <row r="13">
       <c r="A13" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 10:35:41 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 11:03:19 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2940,7 +2940,7 @@
     <row r="11">
       <c r="A11" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 10:35:41 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 11:03:19 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: remove debug words
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -240,7 +240,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -265,7 +265,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -290,7 +290,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -315,7 +315,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -340,7 +340,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -365,7 +365,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -390,7 +390,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -415,7 +415,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -445,7 +445,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -470,7 +470,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -495,7 +495,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -520,7 +520,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -545,7 +545,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -570,7 +570,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -595,7 +595,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -620,7 +620,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -645,7 +645,7 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="9" name="Image 9" descr="Picture"/>
@@ -675,7 +675,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -700,7 +700,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -725,7 +725,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -750,7 +750,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -775,7 +775,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -800,7 +800,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -825,7 +825,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -855,7 +855,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -880,7 +880,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -905,7 +905,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -930,7 +930,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -955,7 +955,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -985,7 +985,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1010,7 +1010,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -1035,7 +1035,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2286000" cy="762000"/>
+    <ext cx="1714500" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -1680,7 +1680,7 @@
     <row r="16">
       <c r="A16" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 11:03:18 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 13:37:11 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
     <row r="17">
       <c r="A17" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 11:03:18 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 13:37:11 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2414,7 +2414,7 @@
     <row r="15">
       <c r="A15" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 11:03:19 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 13:37:11 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2703,7 +2703,7 @@
     <row r="13">
       <c r="A13" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 11:03:19 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 13:37:12 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2940,7 +2940,7 @@
     <row r="11">
       <c r="A11" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 11:03:19 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 13:37:12 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update sheet styles
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -43,17 +43,17 @@
     <font>
       <name val="Calibri"/>
       <b val="1"/>
-      <sz val="14"/>
+      <sz val="16"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="11"/>
+      <sz val="14"/>
     </font>
     <font>
       <name val="Calibri"/>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
-      <sz val="12"/>
+      <sz val="14"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -71,7 +71,7 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="9"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="5">
@@ -240,7 +240,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -265,7 +265,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -290,7 +290,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -315,7 +315,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -340,7 +340,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -365,7 +365,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -390,7 +390,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -415,7 +415,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -445,7 +445,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -470,7 +470,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -495,7 +495,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -520,7 +520,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -545,7 +545,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -570,7 +570,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -595,7 +595,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -620,7 +620,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -645,7 +645,7 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="9" name="Image 9" descr="Picture"/>
@@ -675,7 +675,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -700,7 +700,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -725,7 +725,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -750,7 +750,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -775,7 +775,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -800,7 +800,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -825,7 +825,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -855,7 +855,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -880,7 +880,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -905,7 +905,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -930,7 +930,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -955,7 +955,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -985,7 +985,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1010,7 +1010,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -1035,7 +1035,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1714500" cy="952500"/>
+    <ext cx="3333750" cy="1143000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -1356,12 +1356,12 @@
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="45" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -1680,7 +1680,7 @@
     <row r="16">
       <c r="A16" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 13:37:11 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -1723,12 +1723,12 @@
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="45" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -2073,7 +2073,7 @@
     <row r="17">
       <c r="A17" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 13:37:11 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2116,12 +2116,12 @@
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="45" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -2414,7 +2414,7 @@
     <row r="15">
       <c r="A15" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 13:37:11 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2457,12 +2457,12 @@
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="45" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -2703,7 +2703,7 @@
     <row r="13">
       <c r="A13" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 13:37:12 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2746,12 +2746,12 @@
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="45" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -2940,7 +2940,7 @@
     <row r="11">
       <c r="A11" s="11" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-13 13:37:12 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-13 15:09:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: divide graphic python files
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -74,7 +74,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -85,12 +85,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="004A90E2"/>
         <bgColor rgb="004A90E2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F8F9FA"/>
-        <bgColor rgb="00F8F9FA"/>
       </patternFill>
     </fill>
     <fill>
@@ -124,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -139,11 +133,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1447,26 +1437,26 @@
       </c>
     </row>
     <row r="5" ht="90" customHeight="1">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>#10</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr"/>
-      <c r="D5" s="6" t="n">
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
         <v>3000</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="4" t="n">
         <v>19212</v>
       </c>
-      <c r="G5" s="6" t="inlineStr"/>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>#10-1000+1000+1000x1</t>
         </is>
@@ -1499,26 +1489,26 @@
       </c>
     </row>
     <row r="7" ht="90" customHeight="1">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>#10</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr"/>
-      <c r="D7" s="6" t="n">
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="4" t="n">
         <v>1400</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="4" t="n">
         <v>8966</v>
       </c>
-      <c r="G7" s="6" t="inlineStr"/>
-      <c r="H7" s="6" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>#10-1400x1</t>
         </is>
@@ -1551,26 +1541,26 @@
       </c>
     </row>
     <row r="9" ht="90" customHeight="1">
-      <c r="A9" s="6" t="n">
+      <c r="A9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>#10</t>
         </is>
       </c>
-      <c r="C9" s="7" t="inlineStr"/>
-      <c r="D9" s="6" t="n">
+      <c r="C9" s="5" t="inlineStr"/>
+      <c r="D9" s="4" t="n">
         <v>510</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="4" t="n">
         <v>3269</v>
       </c>
-      <c r="G9" s="6" t="inlineStr"/>
-      <c r="H9" s="6" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t>#10-510.5x11</t>
         </is>
@@ -1603,84 +1593,84 @@
       </c>
     </row>
     <row r="11" ht="90" customHeight="1">
-      <c r="A11" s="6" t="n">
+      <c r="A11" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>#10</t>
         </is>
       </c>
-      <c r="C11" s="7" t="inlineStr"/>
-      <c r="D11" s="6" t="n">
+      <c r="C11" s="5" t="inlineStr"/>
+      <c r="D11" s="4" t="n">
         <v>2000</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="4" t="n">
         <v>12808</v>
       </c>
-      <c r="G11" s="6" t="inlineStr"/>
-      <c r="H11" s="6" t="inlineStr">
+      <c r="G11" s="4" t="inlineStr"/>
+      <c r="H11" s="4" t="inlineStr">
         <is>
           <t>#10-1000+1000x7</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>統計摘要</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="inlineStr">
+      <c r="A14" s="7" t="inlineStr">
         <is>
           <t>總數量</t>
         </is>
       </c>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>63 支</t>
         </is>
       </c>
-      <c r="C14" s="9" t="inlineStr">
+      <c r="C14" s="7" t="inlineStr">
         <is>
           <t>總重量</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D14" s="8" t="inlineStr">
         <is>
           <t>65658.00 kg</t>
         </is>
       </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="E14" s="7" t="inlineStr">
         <is>
           <t>總長度</t>
         </is>
       </c>
-      <c r="F14" s="10" t="inlineStr">
+      <c r="F14" s="8" t="inlineStr">
         <is>
           <t>125491 cm</t>
         </is>
       </c>
-      <c r="G14" s="9" t="inlineStr">
+      <c r="G14" s="7" t="inlineStr">
         <is>
           <t>鋼筋類型</t>
         </is>
       </c>
-      <c r="H14" s="10" t="inlineStr">
+      <c r="H14" s="8" t="inlineStr">
         <is>
           <t>2 種</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+      <c r="A16" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-20 16:00:14 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -1814,26 +1804,26 @@
       </c>
     </row>
     <row r="5" ht="90" customHeight="1">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>#9</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr"/>
-      <c r="D5" s="6" t="n">
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="4" t="n">
         <v>1508</v>
       </c>
-      <c r="G5" s="6" t="inlineStr"/>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>#9-300x1</t>
         </is>
@@ -1866,26 +1856,26 @@
       </c>
     </row>
     <row r="7" ht="90" customHeight="1">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>#7</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr"/>
-      <c r="D7" s="6" t="n">
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="4" t="n">
         <v>913</v>
       </c>
-      <c r="G7" s="6" t="inlineStr"/>
-      <c r="H7" s="6" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>#7-300x1</t>
         </is>
@@ -1918,26 +1908,26 @@
       </c>
     </row>
     <row r="9" ht="90" customHeight="1">
-      <c r="A9" s="6" t="n">
+      <c r="A9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>#5</t>
         </is>
       </c>
-      <c r="C9" s="7" t="inlineStr"/>
-      <c r="D9" s="6" t="n">
+      <c r="C9" s="5" t="inlineStr"/>
+      <c r="D9" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="4" t="n">
         <v>466</v>
       </c>
-      <c r="G9" s="6" t="inlineStr"/>
-      <c r="H9" s="6" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t>#5-300x1</t>
         </is>
@@ -1970,26 +1960,26 @@
       </c>
     </row>
     <row r="11" ht="90" customHeight="1">
-      <c r="A11" s="6" t="n">
+      <c r="A11" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>#10</t>
         </is>
       </c>
-      <c r="C11" s="7" t="inlineStr"/>
-      <c r="D11" s="6" t="n">
+      <c r="C11" s="5" t="inlineStr"/>
+      <c r="D11" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="4" t="n">
         <v>1921</v>
       </c>
-      <c r="G11" s="6" t="inlineStr"/>
-      <c r="H11" s="6" t="inlineStr">
+      <c r="G11" s="4" t="inlineStr"/>
+      <c r="H11" s="4" t="inlineStr">
         <is>
           <t>#10-300x1</t>
         </is>
@@ -2022,58 +2012,58 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>統計摘要</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="inlineStr">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>總數量</t>
         </is>
       </c>
-      <c r="B15" s="10" t="inlineStr">
+      <c r="B15" s="8" t="inlineStr">
         <is>
           <t>9 支</t>
         </is>
       </c>
-      <c r="C15" s="9" t="inlineStr">
+      <c r="C15" s="7" t="inlineStr">
         <is>
           <t>總重量</t>
         </is>
       </c>
-      <c r="D15" s="10" t="inlineStr">
+      <c r="D15" s="8" t="inlineStr">
         <is>
           <t>9509.00 kg</t>
         </is>
       </c>
-      <c r="E15" s="9" t="inlineStr">
+      <c r="E15" s="7" t="inlineStr">
         <is>
           <t>總長度</t>
         </is>
       </c>
-      <c r="F15" s="10" t="inlineStr">
+      <c r="F15" s="8" t="inlineStr">
         <is>
           <t>2700 cm</t>
         </is>
       </c>
-      <c r="G15" s="9" t="inlineStr">
+      <c r="G15" s="7" t="inlineStr">
         <is>
           <t>鋼筋類型</t>
         </is>
       </c>
-      <c r="H15" s="10" t="inlineStr">
+      <c r="H15" s="8" t="inlineStr">
         <is>
           <t>9 種</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+      <c r="A17" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2207,26 +2197,26 @@
       </c>
     </row>
     <row r="5" ht="90" customHeight="1">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>#11</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr"/>
-      <c r="D5" s="6" t="n">
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="4" t="n">
         <v>3953</v>
       </c>
-      <c r="G5" s="6" t="inlineStr"/>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>#11-500x1</t>
         </is>
@@ -2259,26 +2249,26 @@
       </c>
     </row>
     <row r="7" ht="90" customHeight="1">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>#11</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr"/>
-      <c r="D7" s="6" t="n">
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="4" t="n">
         <v>560</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="4" t="n">
         <v>4427</v>
       </c>
-      <c r="G7" s="6" t="inlineStr"/>
-      <c r="H7" s="6" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>#11-60+500x1</t>
         </is>
@@ -2311,26 +2301,26 @@
       </c>
     </row>
     <row r="9" ht="90" customHeight="1">
-      <c r="A9" s="6" t="n">
+      <c r="A9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>#11</t>
         </is>
       </c>
-      <c r="C9" s="7" t="inlineStr"/>
-      <c r="D9" s="6" t="n">
+      <c r="C9" s="5" t="inlineStr"/>
+      <c r="D9" s="4" t="n">
         <v>1120</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="4" t="n">
         <v>8855</v>
       </c>
-      <c r="G9" s="6" t="inlineStr"/>
-      <c r="H9" s="6" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t>#11-60+1000+60x1</t>
         </is>
@@ -2363,58 +2353,58 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>統計摘要</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="inlineStr">
+      <c r="A13" s="7" t="inlineStr">
         <is>
           <t>總數量</t>
         </is>
       </c>
-      <c r="B13" s="10" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
         <is>
           <t>7 支</t>
         </is>
       </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="C13" s="7" t="inlineStr">
         <is>
           <t>總重量</t>
         </is>
       </c>
-      <c r="D13" s="10" t="inlineStr">
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>40795.00 kg</t>
         </is>
       </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="E13" s="7" t="inlineStr">
         <is>
           <t>總長度</t>
         </is>
       </c>
-      <c r="F13" s="10" t="inlineStr">
+      <c r="F13" s="8" t="inlineStr">
         <is>
           <t>5160 cm</t>
         </is>
       </c>
-      <c r="G13" s="9" t="inlineStr">
+      <c r="G13" s="7" t="inlineStr">
         <is>
           <t>鋼筋類型</t>
         </is>
       </c>
-      <c r="H13" s="10" t="inlineStr">
+      <c r="H13" s="8" t="inlineStr">
         <is>
           <t>1 種</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+      <c r="A15" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2548,26 +2538,26 @@
       </c>
     </row>
     <row r="5" ht="90" customHeight="1">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>#11</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr"/>
-      <c r="D5" s="6" t="n">
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
         <v>700</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="4" t="n">
         <v>5534</v>
       </c>
-      <c r="G5" s="6" t="inlineStr"/>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>#11-700x1</t>
         </is>
@@ -2600,26 +2590,26 @@
       </c>
     </row>
     <row r="7" ht="90" customHeight="1">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>#9</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr"/>
-      <c r="D7" s="6" t="n">
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="4" t="n">
         <v>745</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="4" t="n">
         <v>3744</v>
       </c>
-      <c r="G7" s="6" t="inlineStr"/>
-      <c r="H7" s="6" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>#9-45+700x50</t>
         </is>
@@ -2652,58 +2642,58 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>統計摘要</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>總數量</t>
         </is>
       </c>
-      <c r="B11" s="10" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
         <is>
           <t>103 支</t>
         </is>
       </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="C11" s="7" t="inlineStr">
         <is>
           <t>總重量</t>
         </is>
       </c>
-      <c r="D11" s="10" t="inlineStr">
+      <c r="D11" s="8" t="inlineStr">
         <is>
           <t>24090.00 kg</t>
         </is>
       </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr">
         <is>
           <t>總長度</t>
         </is>
       </c>
-      <c r="F11" s="10" t="inlineStr">
+      <c r="F11" s="8" t="inlineStr">
         <is>
           <t>76600 cm</t>
         </is>
       </c>
-      <c r="G11" s="9" t="inlineStr">
+      <c r="G11" s="7" t="inlineStr">
         <is>
           <t>鋼筋類型</t>
         </is>
       </c>
-      <c r="H11" s="10" t="inlineStr">
+      <c r="H11" s="8" t="inlineStr">
         <is>
           <t>2 種</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-13 15:09:04 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+      <c r="A13" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2837,26 +2827,26 @@
       </c>
     </row>
     <row r="5" ht="90" customHeight="1">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>#11</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr"/>
-      <c r="D5" s="6" t="n">
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
         <v>660</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="4" t="n">
         <v>5218</v>
       </c>
-      <c r="G5" s="6" t="inlineStr"/>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>#11-60+600x10</t>
         </is>
@@ -2889,58 +2879,58 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>統計摘要</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>總數量</t>
         </is>
       </c>
-      <c r="B9" s="10" t="inlineStr">
+      <c r="B9" s="8" t="inlineStr">
         <is>
           <t>25 支</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C9" s="7" t="inlineStr">
         <is>
           <t>總重量</t>
         </is>
       </c>
-      <c r="D9" s="10" t="inlineStr">
+      <c r="D9" s="8" t="inlineStr">
         <is>
           <t>15654.00 kg</t>
         </is>
       </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="E9" s="7" t="inlineStr">
         <is>
           <t>總長度</t>
         </is>
       </c>
-      <c r="F9" s="10" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>16200 cm</t>
         </is>
       </c>
-      <c r="G9" s="9" t="inlineStr">
+      <c r="G9" s="7" t="inlineStr">
         <is>
           <t>鋼筋類型</t>
         </is>
       </c>
-      <c r="H9" s="10" t="inlineStr">
+      <c r="H9" s="8" t="inlineStr">
         <is>
           <t>1 種</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-13 15:09:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+      <c r="A11" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: read and write stirrup shape
</commit_message>
<xml_diff>
--- a/assets/example1/example1.xlsx
+++ b/assets/example1/example1.xlsx
@@ -1670,7 +1670,7 @@
     <row r="16">
       <c r="A16" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 16:00:14 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:09:02 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
     <row r="17">
       <c r="A17" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:09:03 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2404,7 +2404,7 @@
     <row r="15">
       <c r="A15" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:09:03 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2693,7 +2693,7 @@
     <row r="13">
       <c r="A13" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:09:03 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -2930,7 +2930,7 @@
     <row r="11">
       <c r="A11" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 16:00:15 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:09:03 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>

</xml_diff>